<commit_message>
Fixed bug in models
</commit_message>
<xml_diff>
--- a/inst/models/SEIR.xlsx
+++ b/inst/models/SEIR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -106,9 +106,6 @@
     <t xml:space="preserve">t * I/(S+E+I+R) * S</t>
   </si>
   <si>
-    <t xml:space="preserve">-t</t>
-  </si>
-  <si>
     <t xml:space="preserve">infect</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t xml:space="preserve">i * E</t>
   </si>
   <si>
-    <t xml:space="preserve">-i</t>
-  </si>
-  <si>
     <t xml:space="preserve">recover</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">r * I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-r</t>
   </si>
 </sst>
 </file>
@@ -242,7 +233,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
   </cols>
@@ -335,11 +326,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.98"/>
   </cols>
@@ -383,7 +374,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,7 +388,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -422,7 +413,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -464,11 +455,11 @@
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.06"/>
@@ -515,11 +506,11 @@
       <c r="D2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
+      <c r="E2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>0</v>
@@ -530,25 +521,25 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
+      <c r="F3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
@@ -556,16 +547,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>0</v>
@@ -573,11 +564,11 @@
       <c r="F4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>18</v>
+      <c r="G4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Definition of functions now included in workbook
</commit_message>
<xml_diff>
--- a/inst/models/SEIR.xlsx
+++ b/inst/models/SEIR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -85,10 +85,13 @@
     <t xml:space="preserve">recovery rate constant</t>
   </si>
   <si>
+    <t xml:space="preserve">code</t>
+  </si>
+  <si>
     <t xml:space="preserve">dummy</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
+    <t xml:space="preserve">dummy &lt;- function() { NULL }</t>
   </si>
   <si>
     <t xml:space="preserve">rate</t>
@@ -132,7 +135,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -154,13 +157,26 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -197,8 +213,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -219,6 +239,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -229,11 +309,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
   </cols>
@@ -248,46 +328,46 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>80000000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>800000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -295,13 +375,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -326,13 +406,13 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -345,18 +425,18 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -364,13 +444,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -378,13 +458,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -410,32 +490,31 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.39"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -456,15 +535,15 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="3.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="8.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="2" width="3.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -494,80 +573,80 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="G2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="n">
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="n">
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="2" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>